<commit_message>
Bug in FuzzDataInserter.exe. Also excluded data with blanks for fairer evaluation.
</commit_message>
<xml_diff>
--- a/PLDI-2012/raw_data/fuzz2/fuzzed/fanniemae_fuzzed_0.xlsx
+++ b/PLDI-2012/raw_data/fuzz2/fuzzed/fanniemae_fuzzed_0.xlsx
@@ -1391,7 +1391,8 @@
         <v>19</v>
       </c>
       <c r="C18" s="1">
-        <v>1515501800</v>
+        <f>SUM(C12:C17)</f>
+        <v>1619075017.7799997</v>
       </c>
       <c r="D18" s="1">
         <f>SUM(D12:D17)</f>
@@ -1505,7 +1506,8 @@
         <v>22</v>
       </c>
       <c r="C21" s="33">
-        <v>1124090364</v>
+        <f>SUM(C18:C20)</f>
+        <v>2013063582.0599997</v>
       </c>
       <c r="D21" s="33">
         <f>SUM(D18:D20)</f>
@@ -1584,7 +1586,7 @@
       </c>
       <c r="C23" s="33">
         <f>SUM(C21:C22)</f>
-        <v>1157466459</v>
+        <v>2046439677.0599997</v>
       </c>
       <c r="D23" s="33">
         <f>SUM(D21:D22)</f>
@@ -1632,7 +1634,7 @@
       </c>
       <c r="C25" s="5">
         <f>C23/C26</f>
-        <v>1.1535807134994533</v>
+        <v>2.0395695481630067</v>
       </c>
       <c r="D25" s="5">
         <f>D23/D26</f>
@@ -1727,7 +1729,7 @@
       <c r="C28" s="6"/>
       <c r="D28" s="16">
         <f>(D25-C25)/C25</f>
-        <v>-8.6157680835953321E-2</v>
+        <v>-0.4831307049486292</v>
       </c>
       <c r="E28" s="16">
         <f>(E25-D25)/D25</f>
@@ -1763,7 +1765,7 @@
       </c>
       <c r="C29" s="5">
         <f>SUM(C25:G25)/5</f>
-        <v>1.0332873086795469</v>
+        <v>1.2104850756122576</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="12"/>

</xml_diff>